<commit_message>
all totals and spreads
</commit_message>
<xml_diff>
--- a/backend/data/odds/2021/Week_16.xlsx
+++ b/backend/data/odds/2021/Week_16.xlsx
@@ -471,22 +471,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Chargers</t>
+          <t>Titans</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Chiefs</t>
+          <t>49ers</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+150</t>
+          <t>+145</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-170</t>
+          <t>-165</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -502,22 +502,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Colts</t>
+          <t>Packers</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Patriots</t>
+          <t>Browns</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-120</t>
+          <t>-380</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>+100</t>
+          <t>+290</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -533,22 +533,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bills</t>
+          <t>Cardinals</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Panthers</t>
+          <t>Colts</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-900</t>
+          <t>-120</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>+600</t>
+          <t>+100</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -564,22 +564,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dolphins</t>
+          <t>Falcons</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Jets</t>
+          <t>Lions</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-475</t>
+          <t>-250</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>+350</t>
+          <t>+200</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -595,22 +595,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lions</t>
+          <t>Bengals</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Cardinals</t>
+          <t>Ravens</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+525</t>
+          <t>-140</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-760</t>
+          <t>+120</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -626,22 +626,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Giants</t>
+          <t>Vikings</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cowboys</t>
+          <t>Rams</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>+425</t>
+          <t>+135</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-590</t>
+          <t>-155</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -657,22 +657,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Steelers</t>
+          <t>Patriots</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Titans</t>
+          <t>Bills</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-120</t>
+          <t>-140</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>+100</t>
+          <t>+120</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -688,22 +688,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Jets</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>Jaguars</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Texans</t>
-        </is>
-      </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>-265</t>
+          <t>-110</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>+215</t>
+          <t>-110</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -719,22 +719,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Broncos</t>
+          <t>Eagles</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bengals</t>
+          <t>Giants</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>-135</t>
+          <t>-475</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>+115</t>
+          <t>+350</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -750,22 +750,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>49ers</t>
+          <t>Panthers</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Falcons</t>
+          <t>Buccaneers</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>-425</t>
+          <t>+340</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>+320</t>
+          <t>-450</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -781,22 +781,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ravens</t>
+          <t>Texans</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Packers</t>
+          <t>Chargers</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>+310</t>
+          <t>+350</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-410</t>
+          <t>-475</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -812,22 +812,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Buccaneers</t>
+          <t>Seahawks</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Saints</t>
+          <t>Bears</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>-630</t>
+          <t>-275</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>+450</t>
+          <t>+220</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -843,22 +843,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Browns</t>
+          <t>Chiefs</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Raiders</t>
+          <t>Steelers</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>+125</t>
+          <t>-350</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>-145</t>
+          <t>+270</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -874,22 +874,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bears</t>
+          <t>Raiders</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Vikings</t>
+          <t>Broncos</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>+240</t>
+          <t>-110</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>-305</t>
+          <t>-110</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Eagles</t>
+          <t>Cowboys</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -936,22 +936,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Rams</t>
+          <t>Saints</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Seahawks</t>
+          <t>Dolphins</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>-350</t>
+          <t>-160</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>+270</t>
+          <t>+140</t>
         </is>
       </c>
       <c r="F17" t="n">

</xml_diff>